<commit_message>
Proyecto Procesos, con persistencia de Datos, falta persistencia en pedidos.
</commit_message>
<xml_diff>
--- a/prueba_escritura.xlsx
+++ b/prueba_escritura.xlsx
@@ -1,100 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c7fdd481179cc1/Escritorio/algordanza_procesos/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_6A69C497014A5AC186E115D24F1510344D07F1FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D9B547D-2FD1-4E2B-87B5-C2F87946FEED}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="3870" windowWidth="23250" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Pedidos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Correo</t>
-  </si>
-  <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>Liana</t>
-  </si>
-  <si>
-    <t>liana@gmail.com</t>
-  </si>
-  <si>
-    <t>Cartagena</t>
-  </si>
-  <si>
-    <t>Pacho</t>
-  </si>
-  <si>
-    <t>pachito@outlook.com</t>
-  </si>
-  <si>
-    <t>Buenaventura</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Juanesxd@gmail.com</t>
-  </si>
-  <si>
-    <t>Medellin</t>
-  </si>
-  <si>
-    <t>Chuchito</t>
-  </si>
-  <si>
-    <t>chuchito@soyudemedellin.edu.co</t>
-  </si>
-  <si>
-    <t>Maria Clara</t>
-  </si>
-  <si>
-    <t>mc@unal.edu.co</t>
-  </si>
-  <si>
-    <t>300896784</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -113,21 +48,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -415,122 +409,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Correo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ciudad</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Celular</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Juanes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>jvaldeso@unal.edu.co</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3007900588</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cristian</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>cristian@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>145464231</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>300048454</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>676576487</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>3007900588</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>300456786</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Id_cliente</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Id_Pedido</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Productos</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Obteniendo valores de del striing productos y falta cargar informacion pedidos.
</commit_message>
<xml_diff>
--- a/prueba_escritura.xlsx
+++ b/prueba_escritura.xlsx
@@ -1,35 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c7fdd481179cc1/Escritorio/algordanza_procesos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_67D52AEBDF5C5DC45FB1195539B49296C2BD1FD4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6FA4762-E8F8-418C-BAAC-BFA0AEC2CE6C}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2325" yWindow="2085" windowWidth="23250" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Pedidos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Pedidos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>Juanes</t>
+  </si>
+  <si>
+    <t>jvaldeso@unal.edu.co</t>
+  </si>
+  <si>
+    <t>Medellin</t>
+  </si>
+  <si>
+    <t>Cristian</t>
+  </si>
+  <si>
+    <t>cristian@gmail.com</t>
+  </si>
+  <si>
+    <t>Id_cliente</t>
+  </si>
+  <si>
+    <t>Id_Pedido</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El tamaño del Diamante es 0.4 
+El grabado del Diamante es True 
+El origen del diamante es Cabello 
+El corte del diamante es Princesa 
+El tamaño del Diamante es 0.5 
+El grabado del Diamante es True 
+El origen del diamante es Cenizas 
+</t>
+  </si>
+  <si>
+    <t>2003-04-20 00:00:00</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,81 +111,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -409,92 +417,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Correo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Ciudad</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Celular</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Juanes</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>jvaldeso@unal.edu.co</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Medellin</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
         <v>3007900588</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Cristian</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>cristian@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Medellin</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>145464231</t>
-        </is>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>145464231</v>
       </c>
     </row>
   </sheetData>
@@ -503,39 +481,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Id_cliente</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Id_Pedido</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Productos</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se hizo funcion para a través de string largo pedidos, obtener solo los valores necesarios en string. Ya se logro la persistencia de la información de los pedidos.
</commit_message>
<xml_diff>
--- a/prueba_escritura.xlsx
+++ b/prueba_escritura.xlsx
@@ -1,99 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c7fdd481179cc1/Escritorio/algordanza_procesos/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_67D52AEBDF5C5DC45FB1195539B49296C2BD1FD4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6FA4762-E8F8-418C-BAAC-BFA0AEC2CE6C}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="2085" windowWidth="23250" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Pedidos" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Pedidos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Correo</t>
-  </si>
-  <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>Juanes</t>
-  </si>
-  <si>
-    <t>jvaldeso@unal.edu.co</t>
-  </si>
-  <si>
-    <t>Medellin</t>
-  </si>
-  <si>
-    <t>Cristian</t>
-  </si>
-  <si>
-    <t>cristian@gmail.com</t>
-  </si>
-  <si>
-    <t>Id_cliente</t>
-  </si>
-  <si>
-    <t>Id_Pedido</t>
-  </si>
-  <si>
-    <t>Productos</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El tamaño del Diamante es 0.4 
-El grabado del Diamante es True 
-El origen del diamante es Cabello 
-El corte del diamante es Princesa 
-El tamaño del Diamante es 0.5 
-El grabado del Diamante es True 
-El origen del diamante es Cenizas 
-</t>
-  </si>
-  <si>
-    <t>2003-04-20 00:00:00</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -111,25 +47,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -417,62 +409,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Correo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ciudad</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Celular</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Juanes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>jvaldeso@unal.edu.co</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3007900588</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cristian</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>cristian@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>145464231</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Chucho</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>3007900588</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>145464231</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>chucho@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3007900588</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -481,41 +526,90 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Id_cliente</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Id_Pedido</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Productos</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El tamaño del Diamante es 0.7 
+El grabado del Diamante es True 
+El origen del diamante es Cabello 
+El tamaño del Diamante es 0.4 
+El grabado del Diamante es True 
+El origen del diamante es Cabello 
+El corte del diamante es Princesa 
+</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20/04/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El tamaño del Diamante es 0.6 
+El grabado del Diamante es True 
+El origen del diamante es Cenizas 
+El corte del diamante es Esmeralda 
+El tamaño del Diamante es 0.4 
+El grabado del Diamante es True 
+El origen del diamante es Mascota 
+El corte del diamante es Asscher 
+</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>20/04/2022</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>